<commit_message>
Some modifications to the file Test_Plan.xls
</commit_message>
<xml_diff>
--- a/testing/V-Cycle Process/V_Cycle Process Script.xlsx
+++ b/testing/V-Cycle Process/V_Cycle Process Script.xlsx
@@ -5,11 +5,11 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hp\Documents\Gilberto Work Space (Window Lifter)\testing\V-Cycle Process\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hp\Documents\Continental AEP\Gilberto Work Space (Window Lifter)\trunk\testing\V-Cycle Process\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
   </bookViews>
   <sheets>
     <sheet name="V-Cycle" sheetId="2" r:id="rId1"/>
@@ -1993,7 +1993,7 @@
   <sheetPr codeName="Hoja1"/>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
@@ -2008,7 +2008,7 @@
   <sheetPr codeName="Hoja2"/>
   <dimension ref="C2:E33"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>

</xml_diff>